<commit_message>
fixed season numbering for season 16
</commit_message>
<xml_diff>
--- a/data/episodes/season_numbering.xlsx
+++ b/data/episodes/season_numbering.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>S.</t>
   </si>
@@ -69,16 +69,7 @@
     <t xml:space="preserve">BW: Rival Destinies</t>
   </si>
   <si>
-    <t xml:space="preserve">16 a</t>
-  </si>
-  <si>
     <t xml:space="preserve">BW: Adventures in Unova</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adventures in Unova and Beyond</t>
   </si>
   <si>
     <t>XY</t>
@@ -4039,11 +4030,11 @@
       <c r="CG16" s="1"/>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
@@ -4120,27 +4111,69 @@
       <c r="AA17" s="11">
         <v>25</v>
       </c>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="13"/>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="13"/>
-      <c r="AJ17" s="13"/>
-      <c r="AK17" s="13"/>
-      <c r="AL17" s="13"/>
-      <c r="AM17" s="13"/>
-      <c r="AN17" s="13"/>
-      <c r="AO17" s="13"/>
-      <c r="AP17" s="13"/>
-      <c r="AQ17" s="13"/>
-      <c r="AR17" s="13"/>
-      <c r="AS17" s="13"/>
-      <c r="AT17" s="13"/>
-      <c r="AU17" s="13"/>
-      <c r="AV17" s="13"/>
+      <c r="AB17" s="11">
+        <v>26</v>
+      </c>
+      <c r="AC17" s="1">
+        <v>27</v>
+      </c>
+      <c r="AD17" s="10">
+        <v>28</v>
+      </c>
+      <c r="AE17" s="1">
+        <v>29</v>
+      </c>
+      <c r="AF17" s="1">
+        <v>30</v>
+      </c>
+      <c r="AG17" s="7">
+        <v>31</v>
+      </c>
+      <c r="AH17" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI17" s="1">
+        <v>33</v>
+      </c>
+      <c r="AJ17" s="1">
+        <v>34</v>
+      </c>
+      <c r="AK17" s="1">
+        <v>35</v>
+      </c>
+      <c r="AL17" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM17" s="9">
+        <v>16</v>
+      </c>
+      <c r="AN17" s="6">
+        <v>37</v>
+      </c>
+      <c r="AO17" s="1">
+        <v>38</v>
+      </c>
+      <c r="AP17" s="1">
+        <v>39</v>
+      </c>
+      <c r="AQ17" s="1">
+        <v>40</v>
+      </c>
+      <c r="AR17" s="1">
+        <v>41</v>
+      </c>
+      <c r="AS17" s="1">
+        <v>42</v>
+      </c>
+      <c r="AT17" s="1">
+        <v>43</v>
+      </c>
+      <c r="AU17" s="6">
+        <v>44</v>
+      </c>
+      <c r="AV17" s="11">
+        <v>45</v>
+      </c>
       <c r="AW17" s="13"/>
       <c r="AX17" s="13"/>
       <c r="AY17" s="13"/>
@@ -4180,31 +4213,31 @@
       <c r="CG17" s="1"/>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
-        <v>19</v>
+      <c r="A18" s="1">
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="11">
+        <v>18</v>
+      </c>
+      <c r="C18" s="6">
         <v>1</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="5">
         <v>2</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E18" s="5">
         <v>3</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="7">
         <v>4</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="8">
         <v>5</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="8">
         <v>6</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="6">
         <v>7</v>
       </c>
       <c r="J18" s="1">
@@ -4213,70 +4246,126 @@
       <c r="K18" s="1">
         <v>9</v>
       </c>
-      <c r="L18" s="1">
+      <c r="L18" s="7">
         <v>10</v>
       </c>
-      <c r="M18" s="1">
+      <c r="M18" s="7">
         <v>11</v>
       </c>
-      <c r="N18" s="9">
+      <c r="N18" s="1">
+        <v>12</v>
+      </c>
+      <c r="O18" s="1">
+        <v>13</v>
+      </c>
+      <c r="P18" s="1">
+        <v>14</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>15</v>
+      </c>
+      <c r="R18" s="1">
         <v>16</v>
       </c>
-      <c r="O18" s="6">
-        <v>12</v>
-      </c>
-      <c r="P18" s="1">
-        <v>13</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>14</v>
-      </c>
-      <c r="R18" s="1">
-        <v>15</v>
-      </c>
       <c r="S18" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="T18" s="1">
+        <v>18</v>
+      </c>
+      <c r="U18" s="1">
+        <v>19</v>
+      </c>
+      <c r="V18" s="8">
+        <v>20</v>
+      </c>
+      <c r="W18" s="1">
+        <v>21</v>
+      </c>
+      <c r="X18" s="1">
+        <v>22</v>
+      </c>
+      <c r="Y18" s="1">
+        <v>23</v>
+      </c>
+      <c r="Z18" s="8">
+        <v>24</v>
+      </c>
+      <c r="AA18" s="1">
+        <v>25</v>
+      </c>
+      <c r="AB18" s="1">
+        <v>26</v>
+      </c>
+      <c r="AC18" s="11">
+        <v>27</v>
+      </c>
+      <c r="AD18" s="1">
+        <v>28</v>
+      </c>
+      <c r="AE18" s="11">
+        <v>29</v>
+      </c>
+      <c r="AF18" s="11">
+        <v>30</v>
+      </c>
+      <c r="AG18" s="11">
+        <v>31</v>
+      </c>
+      <c r="AH18" s="1">
+        <v>32</v>
+      </c>
+      <c r="AI18" s="11">
+        <v>33</v>
+      </c>
+      <c r="AJ18" s="6">
+        <v>34</v>
+      </c>
+      <c r="AK18" s="5">
+        <v>35</v>
+      </c>
+      <c r="AL18" s="1">
+        <v>36</v>
+      </c>
+      <c r="AM18" s="1">
+        <v>37</v>
+      </c>
+      <c r="AN18" s="12">
         <v>17</v>
       </c>
-      <c r="U18" s="1">
-        <v>18</v>
-      </c>
-      <c r="V18" s="6">
-        <v>19</v>
-      </c>
-      <c r="W18" s="11">
-        <v>20</v>
-      </c>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
-      <c r="AA18" s="13"/>
-      <c r="AB18" s="13"/>
-      <c r="AC18" s="13"/>
-      <c r="AD18" s="13"/>
-      <c r="AE18" s="13"/>
-      <c r="AF18" s="13"/>
-      <c r="AG18" s="13"/>
-      <c r="AH18" s="13"/>
-      <c r="AI18" s="13"/>
-      <c r="AJ18" s="13"/>
-      <c r="AK18" s="13"/>
-      <c r="AL18" s="13"/>
-      <c r="AM18" s="13"/>
-      <c r="AN18" s="13"/>
-      <c r="AO18" s="13"/>
-      <c r="AP18" s="13"/>
-      <c r="AQ18" s="13"/>
-      <c r="AR18" s="13"/>
-      <c r="AS18" s="13"/>
-      <c r="AT18" s="13"/>
-      <c r="AU18" s="13"/>
-      <c r="AV18" s="13"/>
-      <c r="AW18" s="13"/>
-      <c r="AX18" s="13"/>
-      <c r="AY18" s="13"/>
+      <c r="AO18" s="1">
+        <v>38</v>
+      </c>
+      <c r="AP18" s="1">
+        <v>39</v>
+      </c>
+      <c r="AQ18" s="1">
+        <v>40</v>
+      </c>
+      <c r="AR18" s="1">
+        <v>41</v>
+      </c>
+      <c r="AS18" s="1">
+        <v>42</v>
+      </c>
+      <c r="AT18" s="8">
+        <v>43</v>
+      </c>
+      <c r="AU18" s="1">
+        <v>44</v>
+      </c>
+      <c r="AV18" s="1">
+        <v>45</v>
+      </c>
+      <c r="AW18" s="1">
+        <v>46</v>
+      </c>
+      <c r="AX18" s="7">
+        <v>47</v>
+      </c>
+      <c r="AY18" s="1">
+        <v>48</v>
+      </c>
       <c r="AZ18" s="13"/>
       <c r="BA18" s="13"/>
       <c r="BB18" s="13"/>
@@ -4314,30 +4403,30 @@
     </row>
     <row r="19">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="6">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1">
         <v>1</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="1">
         <v>2</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="1">
         <v>3</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="5">
         <v>4</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="1">
         <v>5</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="1">
         <v>6</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <v>7</v>
       </c>
       <c r="J19" s="1">
@@ -4346,94 +4435,94 @@
       <c r="K19" s="1">
         <v>9</v>
       </c>
-      <c r="L19" s="7">
+      <c r="L19" s="8">
         <v>10</v>
       </c>
-      <c r="M19" s="7">
+      <c r="M19" s="1">
         <v>11</v>
       </c>
       <c r="N19" s="1">
         <v>12</v>
       </c>
-      <c r="O19" s="1">
+      <c r="O19" s="5">
         <v>13</v>
       </c>
-      <c r="P19" s="1">
+      <c r="P19" s="7">
         <v>14</v>
       </c>
       <c r="Q19" s="1">
         <v>15</v>
       </c>
-      <c r="R19" s="1">
+      <c r="R19" s="7">
         <v>16</v>
       </c>
-      <c r="S19" s="1">
+      <c r="S19" s="5">
         <v>17</v>
       </c>
       <c r="T19" s="1">
         <v>18</v>
       </c>
-      <c r="U19" s="1">
+      <c r="U19" s="8">
         <v>19</v>
       </c>
-      <c r="V19" s="8">
+      <c r="V19" s="1">
         <v>20</v>
       </c>
       <c r="W19" s="1">
         <v>21</v>
       </c>
-      <c r="X19" s="1">
+      <c r="X19" s="11">
         <v>22</v>
       </c>
       <c r="Y19" s="1">
         <v>23</v>
       </c>
-      <c r="Z19" s="8">
+      <c r="Z19" s="1">
         <v>24</v>
       </c>
       <c r="AA19" s="1">
         <v>25</v>
       </c>
-      <c r="AB19" s="1">
+      <c r="AB19" s="8">
         <v>26</v>
       </c>
-      <c r="AC19" s="11">
+      <c r="AC19" s="7">
         <v>27</v>
       </c>
-      <c r="AD19" s="1">
+      <c r="AD19" s="5">
         <v>28</v>
       </c>
-      <c r="AE19" s="11">
+      <c r="AE19" s="1">
         <v>29</v>
       </c>
-      <c r="AF19" s="11">
+      <c r="AF19" s="1">
         <v>30</v>
       </c>
-      <c r="AG19" s="11">
+      <c r="AG19" s="1">
         <v>31</v>
       </c>
-      <c r="AH19" s="1">
+      <c r="AH19" s="8">
         <v>32</v>
       </c>
-      <c r="AI19" s="11">
+      <c r="AI19" s="1">
         <v>33</v>
       </c>
-      <c r="AJ19" s="6">
+      <c r="AJ19" s="7">
         <v>34</v>
       </c>
-      <c r="AK19" s="5">
+      <c r="AK19" s="12">
+        <v>18</v>
+      </c>
+      <c r="AL19" s="1">
         <v>35</v>
       </c>
-      <c r="AL19" s="1">
+      <c r="AM19" s="1">
         <v>36</v>
       </c>
-      <c r="AM19" s="1">
+      <c r="AN19" s="1">
         <v>37</v>
       </c>
-      <c r="AN19" s="12">
-        <v>17</v>
-      </c>
-      <c r="AO19" s="1">
+      <c r="AO19" s="5">
         <v>38</v>
       </c>
       <c r="AP19" s="1">
@@ -4442,7 +4531,7 @@
       <c r="AQ19" s="1">
         <v>40</v>
       </c>
-      <c r="AR19" s="1">
+      <c r="AR19" s="7">
         <v>41</v>
       </c>
       <c r="AS19" s="1">
@@ -4454,18 +4543,12 @@
       <c r="AU19" s="1">
         <v>44</v>
       </c>
-      <c r="AV19" s="1">
+      <c r="AV19" s="8">
         <v>45</v>
       </c>
-      <c r="AW19" s="1">
-        <v>46</v>
-      </c>
-      <c r="AX19" s="7">
-        <v>47</v>
-      </c>
-      <c r="AY19" s="1">
-        <v>48</v>
-      </c>
+      <c r="AW19" s="13"/>
+      <c r="AX19" s="13"/>
+      <c r="AY19" s="13"/>
       <c r="AZ19" s="13"/>
       <c r="BA19" s="13"/>
       <c r="BB19" s="13"/>
@@ -4503,21 +4586,21 @@
     </row>
     <row r="20">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="1">
+        <v>20</v>
+      </c>
+      <c r="C20" s="11">
         <v>1</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="11">
         <v>2</v>
       </c>
       <c r="E20" s="1">
         <v>3</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="1">
         <v>4</v>
       </c>
       <c r="G20" s="1">
@@ -4529,31 +4612,31 @@
       <c r="I20" s="5">
         <v>7</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="8">
         <v>8</v>
       </c>
       <c r="K20" s="1">
         <v>9</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="1">
         <v>10</v>
       </c>
       <c r="M20" s="1">
         <v>11</v>
       </c>
-      <c r="N20" s="1">
+      <c r="N20" s="7">
         <v>12</v>
       </c>
-      <c r="O20" s="5">
+      <c r="O20" s="11">
         <v>13</v>
       </c>
-      <c r="P20" s="7">
+      <c r="P20" s="1">
         <v>14</v>
       </c>
       <c r="Q20" s="1">
         <v>15</v>
       </c>
-      <c r="R20" s="7">
+      <c r="R20" s="8">
         <v>16</v>
       </c>
       <c r="S20" s="5">
@@ -4565,13 +4648,13 @@
       <c r="U20" s="8">
         <v>19</v>
       </c>
-      <c r="V20" s="1">
+      <c r="V20" s="8">
         <v>20</v>
       </c>
       <c r="W20" s="1">
         <v>21</v>
       </c>
-      <c r="X20" s="11">
+      <c r="X20" s="1">
         <v>22</v>
       </c>
       <c r="Y20" s="1">
@@ -4580,22 +4663,22 @@
       <c r="Z20" s="1">
         <v>24</v>
       </c>
-      <c r="AA20" s="1">
+      <c r="AA20" s="11">
         <v>25</v>
       </c>
-      <c r="AB20" s="8">
+      <c r="AB20" s="1">
         <v>26</v>
       </c>
-      <c r="AC20" s="7">
+      <c r="AC20" s="8">
         <v>27</v>
       </c>
-      <c r="AD20" s="5">
+      <c r="AD20" s="1">
         <v>28</v>
       </c>
-      <c r="AE20" s="1">
+      <c r="AE20" s="8">
         <v>29</v>
       </c>
-      <c r="AF20" s="1">
+      <c r="AF20" s="8">
         <v>30</v>
       </c>
       <c r="AG20" s="1">
@@ -4604,50 +4687,54 @@
       <c r="AH20" s="8">
         <v>32</v>
       </c>
-      <c r="AI20" s="1">
+      <c r="AI20" s="8">
         <v>33</v>
       </c>
-      <c r="AJ20" s="7">
+      <c r="AJ20" s="8">
         <v>34</v>
       </c>
-      <c r="AK20" s="12">
-        <v>18</v>
-      </c>
-      <c r="AL20" s="1">
+      <c r="AK20" s="8">
         <v>35</v>
       </c>
-      <c r="AM20" s="1">
+      <c r="AL20" s="8">
         <v>36</v>
       </c>
-      <c r="AN20" s="1">
+      <c r="AM20" s="8">
         <v>37</v>
       </c>
-      <c r="AO20" s="5">
+      <c r="AN20" s="8">
         <v>38</v>
       </c>
-      <c r="AP20" s="1">
+      <c r="AO20" s="11">
         <v>39</v>
       </c>
-      <c r="AQ20" s="1">
+      <c r="AP20" s="11">
         <v>40</v>
       </c>
-      <c r="AR20" s="7">
+      <c r="AQ20" s="11">
         <v>41</v>
       </c>
-      <c r="AS20" s="1">
+      <c r="AR20" s="11">
         <v>42</v>
       </c>
-      <c r="AT20" s="8">
+      <c r="AS20" s="11">
         <v>43</v>
       </c>
+      <c r="AT20" s="1">
+        <v>44</v>
+      </c>
       <c r="AU20" s="1">
-        <v>44</v>
-      </c>
-      <c r="AV20" s="8">
         <v>45</v>
       </c>
-      <c r="AW20" s="13"/>
-      <c r="AX20" s="13"/>
+      <c r="AV20" s="11">
+        <v>46</v>
+      </c>
+      <c r="AW20" s="6">
+        <v>47</v>
+      </c>
+      <c r="AX20" s="12">
+        <v>19</v>
+      </c>
       <c r="AY20" s="13"/>
       <c r="AZ20" s="13"/>
       <c r="BA20" s="13"/>
@@ -4686,10 +4773,10 @@
     </row>
     <row r="21">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C21" s="11">
         <v>1</v>
@@ -4697,10 +4784,10 @@
       <c r="D21" s="11">
         <v>2</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="11">
         <v>3</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="5">
         <v>4</v>
       </c>
       <c r="G21" s="1">
@@ -4709,16 +4796,16 @@
       <c r="H21" s="1">
         <v>6</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="1">
         <v>7</v>
       </c>
-      <c r="J21" s="8">
+      <c r="J21" s="1">
         <v>8</v>
       </c>
-      <c r="K21" s="1">
+      <c r="K21" s="8">
         <v>9</v>
       </c>
-      <c r="L21" s="1">
+      <c r="L21" s="8">
         <v>10</v>
       </c>
       <c r="M21" s="1">
@@ -4727,31 +4814,31 @@
       <c r="N21" s="7">
         <v>12</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O21" s="7">
         <v>13</v>
       </c>
-      <c r="P21" s="1">
+      <c r="P21" s="7">
         <v>14</v>
       </c>
-      <c r="Q21" s="1">
+      <c r="Q21" s="5">
         <v>15</v>
       </c>
-      <c r="R21" s="8">
+      <c r="R21" s="1">
         <v>16</v>
       </c>
-      <c r="S21" s="5">
+      <c r="S21" s="1">
         <v>17</v>
       </c>
-      <c r="T21" s="1">
+      <c r="T21" s="7">
         <v>18</v>
       </c>
-      <c r="U21" s="8">
+      <c r="U21" s="1">
         <v>19</v>
       </c>
-      <c r="V21" s="8">
+      <c r="V21" s="1">
         <v>20</v>
       </c>
-      <c r="W21" s="1">
+      <c r="W21" s="5">
         <v>21</v>
       </c>
       <c r="X21" s="1">
@@ -4763,34 +4850,34 @@
       <c r="Z21" s="1">
         <v>24</v>
       </c>
-      <c r="AA21" s="11">
+      <c r="AA21" s="1">
         <v>25</v>
       </c>
-      <c r="AB21" s="1">
+      <c r="AB21" s="7">
         <v>26</v>
       </c>
-      <c r="AC21" s="8">
+      <c r="AC21" s="1">
         <v>27</v>
       </c>
       <c r="AD21" s="1">
         <v>28</v>
       </c>
-      <c r="AE21" s="8">
+      <c r="AE21" s="1">
         <v>29</v>
       </c>
-      <c r="AF21" s="8">
+      <c r="AF21" s="1">
         <v>30</v>
       </c>
       <c r="AG21" s="1">
         <v>31</v>
       </c>
-      <c r="AH21" s="8">
+      <c r="AH21" s="1">
         <v>32</v>
       </c>
       <c r="AI21" s="8">
         <v>33</v>
       </c>
-      <c r="AJ21" s="8">
+      <c r="AJ21" s="7">
         <v>34</v>
       </c>
       <c r="AK21" s="8">
@@ -4799,42 +4886,34 @@
       <c r="AL21" s="8">
         <v>36</v>
       </c>
-      <c r="AM21" s="8">
+      <c r="AM21" s="5">
         <v>37</v>
       </c>
-      <c r="AN21" s="8">
+      <c r="AN21" s="1">
         <v>38</v>
       </c>
-      <c r="AO21" s="11">
+      <c r="AO21" s="1">
         <v>39</v>
       </c>
-      <c r="AP21" s="11">
+      <c r="AP21" s="1">
         <v>40</v>
       </c>
-      <c r="AQ21" s="11">
+      <c r="AQ21" s="1">
         <v>41</v>
       </c>
       <c r="AR21" s="11">
         <v>42</v>
       </c>
-      <c r="AS21" s="11">
+      <c r="AS21" s="8">
         <v>43</v>
       </c>
-      <c r="AT21" s="1">
-        <v>44</v>
-      </c>
-      <c r="AU21" s="1">
-        <v>45</v>
-      </c>
-      <c r="AV21" s="11">
-        <v>46</v>
-      </c>
-      <c r="AW21" s="6">
-        <v>47</v>
-      </c>
-      <c r="AX21" s="12">
-        <v>19</v>
-      </c>
+      <c r="AT21" s="12">
+        <v>20</v>
+      </c>
+      <c r="AU21" s="13"/>
+      <c r="AV21" s="13"/>
+      <c r="AW21" s="13"/>
+      <c r="AX21" s="13"/>
       <c r="AY21" s="13"/>
       <c r="AZ21" s="13"/>
       <c r="BA21" s="13"/>
@@ -4873,72 +4952,72 @@
     </row>
     <row r="22">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" s="11">
         <v>1</v>
       </c>
-      <c r="D22" s="11">
+      <c r="D22" s="1">
         <v>2</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22" s="1">
         <v>3</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="11">
         <v>4</v>
       </c>
       <c r="G22" s="1">
         <v>5</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="7">
         <v>6</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="5">
         <v>7</v>
       </c>
       <c r="J22" s="1">
         <v>8</v>
       </c>
-      <c r="K22" s="8">
+      <c r="K22" s="5">
         <v>9</v>
       </c>
-      <c r="L22" s="8">
+      <c r="L22" s="1">
         <v>10</v>
       </c>
       <c r="M22" s="1">
         <v>11</v>
       </c>
-      <c r="N22" s="7">
+      <c r="N22" s="11">
         <v>12</v>
       </c>
-      <c r="O22" s="7">
+      <c r="O22" s="1">
         <v>13</v>
       </c>
-      <c r="P22" s="7">
+      <c r="P22" s="1">
         <v>14</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="Q22" s="1">
         <v>15</v>
       </c>
       <c r="R22" s="1">
         <v>16</v>
       </c>
-      <c r="S22" s="1">
+      <c r="S22" s="7">
         <v>17</v>
       </c>
-      <c r="T22" s="7">
+      <c r="T22" s="1">
         <v>18</v>
       </c>
       <c r="U22" s="1">
         <v>19</v>
       </c>
-      <c r="V22" s="1">
+      <c r="V22" s="5">
         <v>20</v>
       </c>
-      <c r="W22" s="5">
+      <c r="W22" s="1">
         <v>21</v>
       </c>
       <c r="X22" s="1">
@@ -4953,7 +5032,7 @@
       <c r="AA22" s="1">
         <v>25</v>
       </c>
-      <c r="AB22" s="7">
+      <c r="AB22" s="1">
         <v>26</v>
       </c>
       <c r="AC22" s="1">
@@ -4968,31 +5047,31 @@
       <c r="AF22" s="1">
         <v>30</v>
       </c>
-      <c r="AG22" s="1">
+      <c r="AG22" s="8">
         <v>31</v>
       </c>
       <c r="AH22" s="1">
         <v>32</v>
       </c>
-      <c r="AI22" s="8">
+      <c r="AI22" s="1">
         <v>33</v>
       </c>
-      <c r="AJ22" s="7">
+      <c r="AJ22" s="8">
         <v>34</v>
       </c>
-      <c r="AK22" s="8">
+      <c r="AK22" s="1">
         <v>35</v>
       </c>
-      <c r="AL22" s="8">
+      <c r="AL22" s="1">
         <v>36</v>
       </c>
-      <c r="AM22" s="5">
+      <c r="AM22" s="1">
         <v>37</v>
       </c>
       <c r="AN22" s="1">
         <v>38</v>
       </c>
-      <c r="AO22" s="1">
+      <c r="AO22" s="7">
         <v>39</v>
       </c>
       <c r="AP22" s="1">
@@ -5001,20 +5080,30 @@
       <c r="AQ22" s="1">
         <v>41</v>
       </c>
-      <c r="AR22" s="11">
+      <c r="AR22" s="1">
         <v>42</v>
       </c>
-      <c r="AS22" s="8">
+      <c r="AS22" s="1">
         <v>43</v>
       </c>
-      <c r="AT22" s="12">
-        <v>20</v>
-      </c>
-      <c r="AU22" s="13"/>
-      <c r="AV22" s="13"/>
-      <c r="AW22" s="13"/>
-      <c r="AX22" s="13"/>
-      <c r="AY22" s="13"/>
+      <c r="AT22" s="1">
+        <v>44</v>
+      </c>
+      <c r="AU22" s="1">
+        <v>45</v>
+      </c>
+      <c r="AV22" s="1">
+        <v>46</v>
+      </c>
+      <c r="AW22" s="11">
+        <v>47</v>
+      </c>
+      <c r="AX22" s="1">
+        <v>48</v>
+      </c>
+      <c r="AY22" s="1">
+        <v>49</v>
+      </c>
       <c r="AZ22" s="13"/>
       <c r="BA22" s="13"/>
       <c r="BB22" s="13"/>
@@ -5051,13 +5140,13 @@
       <c r="CG22" s="1"/>
     </row>
     <row r="23">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="11">
+      <c r="A23" s="17">
+        <v>22</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="1">
         <v>1</v>
       </c>
       <c r="D23" s="1">
@@ -5066,46 +5155,46 @@
       <c r="E23" s="1">
         <v>3</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="1">
         <v>4</v>
       </c>
       <c r="G23" s="1">
         <v>5</v>
       </c>
-      <c r="H23" s="7">
+      <c r="H23" s="1">
         <v>6</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="7">
         <v>7</v>
       </c>
       <c r="J23" s="1">
         <v>8</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="1">
         <v>9</v>
       </c>
-      <c r="L23" s="1">
+      <c r="L23" s="6">
         <v>10</v>
       </c>
-      <c r="M23" s="1">
+      <c r="M23" s="6">
         <v>11</v>
       </c>
-      <c r="N23" s="11">
+      <c r="N23" s="1">
         <v>12</v>
       </c>
       <c r="O23" s="1">
         <v>13</v>
       </c>
-      <c r="P23" s="1">
+      <c r="P23" s="11">
         <v>14</v>
       </c>
       <c r="Q23" s="1">
         <v>15</v>
       </c>
-      <c r="R23" s="1">
+      <c r="R23" s="11">
         <v>16</v>
       </c>
-      <c r="S23" s="7">
+      <c r="S23" s="8">
         <v>17</v>
       </c>
       <c r="T23" s="1">
@@ -5138,7 +5227,7 @@
       <c r="AC23" s="1">
         <v>27</v>
       </c>
-      <c r="AD23" s="1">
+      <c r="AD23" s="7">
         <v>28</v>
       </c>
       <c r="AE23" s="1">
@@ -5147,7 +5236,7 @@
       <c r="AF23" s="1">
         <v>30</v>
       </c>
-      <c r="AG23" s="8">
+      <c r="AG23" s="1">
         <v>31</v>
       </c>
       <c r="AH23" s="1">
@@ -5156,71 +5245,85 @@
       <c r="AI23" s="1">
         <v>33</v>
       </c>
-      <c r="AJ23" s="8">
+      <c r="AJ23" s="1">
         <v>34</v>
       </c>
-      <c r="AK23" s="1">
+      <c r="AK23" s="7">
         <v>35</v>
       </c>
-      <c r="AL23" s="1">
+      <c r="AL23" s="8">
         <v>36</v>
       </c>
-      <c r="AM23" s="1">
+      <c r="AM23" s="8">
         <v>37</v>
       </c>
-      <c r="AN23" s="1">
+      <c r="AN23" s="8">
         <v>38</v>
       </c>
-      <c r="AO23" s="7">
+      <c r="AO23" s="8">
         <v>39</v>
       </c>
-      <c r="AP23" s="1">
+      <c r="AP23" s="8">
         <v>40</v>
       </c>
-      <c r="AQ23" s="1">
+      <c r="AQ23" s="8">
         <v>41</v>
       </c>
-      <c r="AR23" s="1">
+      <c r="AR23" s="8">
         <v>42</v>
       </c>
-      <c r="AS23" s="1">
+      <c r="AS23" s="8">
         <v>43</v>
       </c>
-      <c r="AT23" s="1">
+      <c r="AT23" s="8">
         <v>44</v>
       </c>
-      <c r="AU23" s="1">
+      <c r="AU23" s="8">
         <v>45</v>
       </c>
-      <c r="AV23" s="1">
+      <c r="AV23" s="8">
         <v>46</v>
       </c>
-      <c r="AW23" s="11">
+      <c r="AW23" s="8">
         <v>47</v>
       </c>
-      <c r="AX23" s="1">
+      <c r="AX23" s="5">
         <v>48</v>
       </c>
-      <c r="AY23" s="1">
+      <c r="AY23" s="8">
         <v>49</v>
       </c>
-      <c r="AZ23" s="13"/>
-      <c r="BA23" s="13"/>
-      <c r="BB23" s="13"/>
-      <c r="BC23" s="13"/>
-      <c r="BD23" s="13"/>
-      <c r="BE23" s="13"/>
-      <c r="BF23" s="13"/>
-      <c r="BG23" s="13"/>
-      <c r="BH23" s="13"/>
-      <c r="BI23" s="13"/>
-      <c r="BJ23" s="13"/>
-      <c r="BK23" s="13"/>
-      <c r="BL23" s="13"/>
-      <c r="BM23" s="13"/>
-      <c r="BN23" s="13"/>
-      <c r="BO23" s="13"/>
-      <c r="BP23" s="13"/>
+      <c r="AZ23" s="8">
+        <v>50</v>
+      </c>
+      <c r="BA23" s="8">
+        <v>51</v>
+      </c>
+      <c r="BB23" s="8">
+        <v>52</v>
+      </c>
+      <c r="BC23" s="15">
+        <v>53</v>
+      </c>
+      <c r="BD23" s="6">
+        <v>54</v>
+      </c>
+      <c r="BE23" s="12">
+        <v>21</v>
+      </c>
+      <c r="BF23" s="12">
+        <v>22</v>
+      </c>
+      <c r="BG23" s="1"/>
+      <c r="BH23" s="1"/>
+      <c r="BI23" s="1"/>
+      <c r="BJ23" s="1"/>
+      <c r="BK23" s="1"/>
+      <c r="BL23" s="1"/>
+      <c r="BM23" s="1"/>
+      <c r="BN23" s="1"/>
+      <c r="BO23" s="1"/>
+      <c r="BP23" s="1"/>
       <c r="BQ23" s="1"/>
       <c r="BR23" s="1"/>
       <c r="BS23" s="1"/>
@@ -5240,189 +5343,175 @@
       <c r="CG23" s="1"/>
     </row>
     <row r="24">
-      <c r="A24" s="17">
+      <c r="A24" s="19">
+        <v>23</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="15">
+        <v>1</v>
+      </c>
+      <c r="D24" s="21">
+        <v>2</v>
+      </c>
+      <c r="E24" s="22">
+        <v>3</v>
+      </c>
+      <c r="F24" s="15">
+        <v>4</v>
+      </c>
+      <c r="G24" s="23">
+        <v>5</v>
+      </c>
+      <c r="H24" s="24">
+        <v>6</v>
+      </c>
+      <c r="I24" s="16">
+        <v>7</v>
+      </c>
+      <c r="J24" s="24">
+        <v>8</v>
+      </c>
+      <c r="K24" s="24">
+        <v>9</v>
+      </c>
+      <c r="L24" s="25">
+        <v>10</v>
+      </c>
+      <c r="M24" s="24">
+        <v>11</v>
+      </c>
+      <c r="N24" s="15">
+        <v>12</v>
+      </c>
+      <c r="O24" s="15">
+        <v>13</v>
+      </c>
+      <c r="P24" s="23">
+        <v>14</v>
+      </c>
+      <c r="Q24" s="24">
+        <v>15</v>
+      </c>
+      <c r="R24" s="25">
+        <v>16</v>
+      </c>
+      <c r="S24" s="23">
+        <v>17</v>
+      </c>
+      <c r="T24" s="16">
+        <v>18</v>
+      </c>
+      <c r="U24" s="24">
+        <v>19</v>
+      </c>
+      <c r="V24" s="16">
+        <v>20</v>
+      </c>
+      <c r="W24" s="25">
+        <v>21</v>
+      </c>
+      <c r="X24" s="22">
         <v>22</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="Y24" s="24">
+        <v>23</v>
+      </c>
+      <c r="Z24" s="24">
+        <v>24</v>
+      </c>
+      <c r="AA24" s="16">
+        <v>25</v>
+      </c>
+      <c r="AB24" s="22">
         <v>26</v>
       </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2</v>
-      </c>
-      <c r="E24" s="1">
-        <v>3</v>
-      </c>
-      <c r="F24" s="1">
-        <v>4</v>
-      </c>
-      <c r="G24" s="1">
-        <v>5</v>
-      </c>
-      <c r="H24" s="1">
-        <v>6</v>
-      </c>
-      <c r="I24" s="7">
-        <v>7</v>
-      </c>
-      <c r="J24" s="1">
-        <v>8</v>
-      </c>
-      <c r="K24" s="1">
-        <v>9</v>
-      </c>
-      <c r="L24" s="6">
-        <v>10</v>
-      </c>
-      <c r="M24" s="6">
-        <v>11</v>
-      </c>
-      <c r="N24" s="1">
-        <v>12</v>
-      </c>
-      <c r="O24" s="1">
-        <v>13</v>
-      </c>
-      <c r="P24" s="11">
-        <v>14</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>15</v>
-      </c>
-      <c r="R24" s="11">
-        <v>16</v>
-      </c>
-      <c r="S24" s="8">
-        <v>17</v>
-      </c>
-      <c r="T24" s="1">
-        <v>18</v>
-      </c>
-      <c r="U24" s="1">
-        <v>19</v>
-      </c>
-      <c r="V24" s="5">
-        <v>20</v>
-      </c>
-      <c r="W24" s="1">
-        <v>21</v>
-      </c>
-      <c r="X24" s="1">
-        <v>22</v>
-      </c>
-      <c r="Y24" s="1">
+      <c r="AC24" s="25">
+        <v>27</v>
+      </c>
+      <c r="AD24" s="23">
+        <v>28</v>
+      </c>
+      <c r="AE24" s="22">
+        <v>29</v>
+      </c>
+      <c r="AF24" s="16">
+        <v>30</v>
+      </c>
+      <c r="AG24" s="24">
+        <v>31</v>
+      </c>
+      <c r="AH24" s="24">
+        <v>32</v>
+      </c>
+      <c r="AI24" s="16">
+        <v>33</v>
+      </c>
+      <c r="AJ24" s="16">
+        <v>34</v>
+      </c>
+      <c r="AK24" s="23">
+        <v>35</v>
+      </c>
+      <c r="AL24" s="16">
+        <v>36</v>
+      </c>
+      <c r="AM24" s="15">
+        <v>37</v>
+      </c>
+      <c r="AN24" s="23">
+        <v>38</v>
+      </c>
+      <c r="AO24" s="16">
+        <v>39</v>
+      </c>
+      <c r="AP24" s="22">
+        <v>40</v>
+      </c>
+      <c r="AQ24" s="22">
+        <v>41</v>
+      </c>
+      <c r="AR24" s="15">
+        <v>42</v>
+      </c>
+      <c r="AS24" s="15">
+        <v>43</v>
+      </c>
+      <c r="AT24" s="15">
+        <v>44</v>
+      </c>
+      <c r="AU24" s="15">
+        <v>45</v>
+      </c>
+      <c r="AV24" s="15">
+        <v>46</v>
+      </c>
+      <c r="AW24" s="24">
+        <v>47</v>
+      </c>
+      <c r="AX24" s="22">
+        <v>48</v>
+      </c>
+      <c r="AY24" s="12">
         <v>23</v>
       </c>
-      <c r="Z24" s="1">
-        <v>24</v>
-      </c>
-      <c r="AA24" s="1">
-        <v>25</v>
-      </c>
-      <c r="AB24" s="1">
-        <v>26</v>
-      </c>
-      <c r="AC24" s="1">
-        <v>27</v>
-      </c>
-      <c r="AD24" s="7">
-        <v>28</v>
-      </c>
-      <c r="AE24" s="1">
-        <v>29</v>
-      </c>
-      <c r="AF24" s="1">
-        <v>30</v>
-      </c>
-      <c r="AG24" s="1">
-        <v>31</v>
-      </c>
-      <c r="AH24" s="1">
-        <v>32</v>
-      </c>
-      <c r="AI24" s="1">
-        <v>33</v>
-      </c>
-      <c r="AJ24" s="1">
-        <v>34</v>
-      </c>
-      <c r="AK24" s="7">
-        <v>35</v>
-      </c>
-      <c r="AL24" s="8">
-        <v>36</v>
-      </c>
-      <c r="AM24" s="8">
-        <v>37</v>
-      </c>
-      <c r="AN24" s="8">
-        <v>38</v>
-      </c>
-      <c r="AO24" s="8">
-        <v>39</v>
-      </c>
-      <c r="AP24" s="8">
-        <v>40</v>
-      </c>
-      <c r="AQ24" s="8">
-        <v>41</v>
-      </c>
-      <c r="AR24" s="8">
-        <v>42</v>
-      </c>
-      <c r="AS24" s="8">
-        <v>43</v>
-      </c>
-      <c r="AT24" s="8">
-        <v>44</v>
-      </c>
-      <c r="AU24" s="8">
-        <v>45</v>
-      </c>
-      <c r="AV24" s="8">
-        <v>46</v>
-      </c>
-      <c r="AW24" s="8">
-        <v>47</v>
-      </c>
-      <c r="AX24" s="5">
-        <v>48</v>
-      </c>
-      <c r="AY24" s="8">
-        <v>49</v>
-      </c>
-      <c r="AZ24" s="8">
-        <v>50</v>
-      </c>
-      <c r="BA24" s="8">
-        <v>51</v>
-      </c>
-      <c r="BB24" s="8">
-        <v>52</v>
-      </c>
-      <c r="BC24" s="15">
-        <v>53</v>
-      </c>
-      <c r="BD24" s="6">
-        <v>54</v>
-      </c>
-      <c r="BE24" s="12">
-        <v>21</v>
-      </c>
-      <c r="BF24" s="12">
-        <v>22</v>
-      </c>
-      <c r="BG24" s="1"/>
-      <c r="BH24" s="1"/>
-      <c r="BI24" s="1"/>
-      <c r="BJ24" s="1"/>
-      <c r="BK24" s="1"/>
-      <c r="BL24" s="1"/>
-      <c r="BM24" s="1"/>
-      <c r="BN24" s="1"/>
-      <c r="BO24" s="1"/>
+      <c r="AZ24" s="13"/>
+      <c r="BA24" s="13"/>
+      <c r="BB24" s="13"/>
+      <c r="BC24" s="13"/>
+      <c r="BD24" s="13"/>
+      <c r="BE24" s="13"/>
+      <c r="BF24" s="13"/>
+      <c r="BG24" s="13"/>
+      <c r="BH24" s="13"/>
+      <c r="BI24" s="13"/>
+      <c r="BJ24" s="13"/>
+      <c r="BK24" s="13"/>
+      <c r="BL24" s="13"/>
+      <c r="BM24" s="13"/>
+      <c r="BN24" s="13"/>
+      <c r="BO24" s="13"/>
       <c r="BP24" s="1"/>
       <c r="BQ24" s="1"/>
       <c r="BR24" s="1"/>
@@ -5444,158 +5533,144 @@
     </row>
     <row r="25">
       <c r="A25" s="19">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="15">
+        <v>25</v>
+      </c>
+      <c r="C25" s="24">
         <v>1</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="25">
         <v>2</v>
       </c>
-      <c r="E25" s="22">
+      <c r="E25" s="16">
         <v>3</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="24">
         <v>4</v>
       </c>
       <c r="G25" s="23">
         <v>5</v>
       </c>
-      <c r="H25" s="24">
+      <c r="H25" s="22">
         <v>6</v>
       </c>
-      <c r="I25" s="16">
+      <c r="I25" s="23">
         <v>7</v>
       </c>
-      <c r="J25" s="24">
+      <c r="J25" s="15">
         <v>8</v>
       </c>
-      <c r="K25" s="24">
+      <c r="K25" s="22">
         <v>9</v>
       </c>
-      <c r="L25" s="25">
+      <c r="L25" s="22">
         <v>10</v>
       </c>
-      <c r="M25" s="24">
+      <c r="M25" s="23">
         <v>11</v>
       </c>
-      <c r="N25" s="15">
+      <c r="N25" s="16">
         <v>12</v>
       </c>
-      <c r="O25" s="15">
+      <c r="O25" s="22">
         <v>13</v>
       </c>
-      <c r="P25" s="23">
+      <c r="P25" s="25">
         <v>14</v>
       </c>
-      <c r="Q25" s="24">
+      <c r="Q25" s="22">
         <v>15</v>
       </c>
-      <c r="R25" s="25">
+      <c r="R25" s="23">
         <v>16</v>
       </c>
-      <c r="S25" s="23">
+      <c r="S25" s="16">
         <v>17</v>
       </c>
-      <c r="T25" s="16">
+      <c r="T25" s="24">
         <v>18</v>
       </c>
-      <c r="U25" s="24">
+      <c r="U25" s="22">
         <v>19</v>
       </c>
-      <c r="V25" s="16">
+      <c r="V25" s="15">
         <v>20</v>
       </c>
-      <c r="W25" s="25">
+      <c r="W25" s="22">
         <v>21</v>
       </c>
-      <c r="X25" s="22">
+      <c r="X25" s="24">
         <v>22</v>
       </c>
-      <c r="Y25" s="24">
+      <c r="Y25" s="23">
         <v>23</v>
       </c>
       <c r="Z25" s="24">
         <v>24</v>
       </c>
-      <c r="AA25" s="16">
+      <c r="AA25" s="24">
         <v>25</v>
       </c>
       <c r="AB25" s="22">
         <v>26</v>
       </c>
-      <c r="AC25" s="25">
+      <c r="AC25" s="22">
         <v>27</v>
       </c>
-      <c r="AD25" s="23">
+      <c r="AD25" s="24">
         <v>28</v>
       </c>
-      <c r="AE25" s="22">
+      <c r="AE25" s="16">
         <v>29</v>
       </c>
-      <c r="AF25" s="16">
+      <c r="AF25" s="23">
         <v>30</v>
       </c>
-      <c r="AG25" s="24">
+      <c r="AG25" s="22">
         <v>31</v>
       </c>
       <c r="AH25" s="24">
         <v>32</v>
       </c>
-      <c r="AI25" s="16">
+      <c r="AI25" s="24">
         <v>33</v>
       </c>
-      <c r="AJ25" s="16">
+      <c r="AJ25" s="24">
         <v>34</v>
       </c>
-      <c r="AK25" s="23">
+      <c r="AK25" s="24">
         <v>35</v>
       </c>
-      <c r="AL25" s="16">
+      <c r="AL25" s="15">
         <v>36</v>
       </c>
-      <c r="AM25" s="15">
+      <c r="AM25" s="16">
         <v>37</v>
       </c>
-      <c r="AN25" s="23">
+      <c r="AN25" s="16">
         <v>38</v>
       </c>
-      <c r="AO25" s="16">
+      <c r="AO25" s="22">
         <v>39</v>
       </c>
-      <c r="AP25" s="22">
+      <c r="AP25" s="24">
         <v>40</v>
       </c>
-      <c r="AQ25" s="22">
+      <c r="AQ25" s="15">
         <v>41</v>
       </c>
       <c r="AR25" s="15">
         <v>42</v>
       </c>
-      <c r="AS25" s="15">
-        <v>43</v>
-      </c>
-      <c r="AT25" s="15">
-        <v>44</v>
-      </c>
-      <c r="AU25" s="15">
-        <v>45</v>
-      </c>
-      <c r="AV25" s="15">
-        <v>46</v>
-      </c>
-      <c r="AW25" s="24">
-        <v>47</v>
-      </c>
-      <c r="AX25" s="22">
-        <v>48</v>
-      </c>
-      <c r="AY25" s="12">
-        <v>23</v>
-      </c>
+      <c r="AS25" s="13"/>
+      <c r="AT25" s="13"/>
+      <c r="AU25" s="13"/>
+      <c r="AV25" s="13"/>
+      <c r="AW25" s="13"/>
+      <c r="AX25" s="13"/>
+      <c r="AY25" s="13"/>
       <c r="AZ25" s="13"/>
       <c r="BA25" s="13"/>
       <c r="BB25" s="13"/>
@@ -5633,10 +5708,10 @@
     </row>
     <row r="26">
       <c r="A26" s="19">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C26" s="24">
         <v>1</v>
@@ -5644,106 +5719,106 @@
       <c r="D26" s="25">
         <v>2</v>
       </c>
-      <c r="E26" s="16">
+      <c r="E26" s="1">
         <v>3</v>
       </c>
       <c r="F26" s="24">
         <v>4</v>
       </c>
-      <c r="G26" s="23">
+      <c r="G26" s="15">
         <v>5</v>
       </c>
-      <c r="H26" s="22">
+      <c r="H26" s="26">
         <v>6</v>
       </c>
-      <c r="I26" s="23">
+      <c r="I26" s="24">
         <v>7</v>
       </c>
-      <c r="J26" s="15">
+      <c r="J26" s="26">
         <v>8</v>
       </c>
-      <c r="K26" s="22">
+      <c r="K26" s="16">
         <v>9</v>
       </c>
-      <c r="L26" s="22">
+      <c r="L26" s="24">
         <v>10</v>
       </c>
-      <c r="M26" s="23">
+      <c r="M26" s="26">
         <v>11</v>
       </c>
-      <c r="N26" s="16">
+      <c r="N26" s="24">
         <v>12</v>
       </c>
-      <c r="O26" s="22">
+      <c r="O26" s="15">
         <v>13</v>
       </c>
-      <c r="P26" s="25">
+      <c r="P26" s="16">
         <v>14</v>
       </c>
-      <c r="Q26" s="22">
+      <c r="Q26" s="16">
         <v>15</v>
       </c>
-      <c r="R26" s="23">
+      <c r="R26" s="26">
         <v>16</v>
       </c>
-      <c r="S26" s="16">
+      <c r="S26" s="26">
         <v>17</v>
       </c>
-      <c r="T26" s="24">
+      <c r="T26" s="23">
         <v>18</v>
       </c>
-      <c r="U26" s="22">
+      <c r="U26" s="16">
         <v>19</v>
       </c>
-      <c r="V26" s="15">
+      <c r="V26" s="26">
         <v>20</v>
       </c>
-      <c r="W26" s="22">
+      <c r="W26" s="26">
         <v>21</v>
       </c>
-      <c r="X26" s="24">
+      <c r="X26" s="26">
         <v>22</v>
       </c>
       <c r="Y26" s="23">
         <v>23</v>
       </c>
-      <c r="Z26" s="24">
+      <c r="Z26" s="15">
         <v>24</v>
       </c>
-      <c r="AA26" s="24">
+      <c r="AA26" s="16">
         <v>25</v>
       </c>
-      <c r="AB26" s="22">
+      <c r="AB26" s="16">
         <v>26</v>
       </c>
-      <c r="AC26" s="22">
+      <c r="AC26" s="16">
         <v>27</v>
       </c>
-      <c r="AD26" s="24">
+      <c r="AD26" s="16">
         <v>28</v>
       </c>
-      <c r="AE26" s="16">
+      <c r="AE26" s="26">
         <v>29</v>
       </c>
-      <c r="AF26" s="23">
+      <c r="AF26" s="26">
         <v>30</v>
       </c>
-      <c r="AG26" s="22">
+      <c r="AG26" s="16">
         <v>31</v>
       </c>
-      <c r="AH26" s="24">
+      <c r="AH26" s="16">
         <v>32</v>
       </c>
-      <c r="AI26" s="24">
+      <c r="AI26" s="16">
         <v>33</v>
       </c>
-      <c r="AJ26" s="24">
+      <c r="AJ26" s="16">
         <v>34</v>
       </c>
-      <c r="AK26" s="24">
+      <c r="AK26" s="16">
         <v>35</v>
       </c>
-      <c r="AL26" s="15">
+      <c r="AL26" s="16">
         <v>36</v>
       </c>
       <c r="AM26" s="16">
@@ -5752,22 +5827,30 @@
       <c r="AN26" s="16">
         <v>38</v>
       </c>
-      <c r="AO26" s="22">
+      <c r="AO26" s="8">
         <v>39</v>
       </c>
-      <c r="AP26" s="24">
+      <c r="AP26" s="8">
         <v>40</v>
       </c>
-      <c r="AQ26" s="15">
+      <c r="AQ26" s="8">
         <v>41</v>
       </c>
-      <c r="AR26" s="15">
+      <c r="AR26" s="8">
         <v>42</v>
       </c>
-      <c r="AS26" s="13"/>
-      <c r="AT26" s="13"/>
-      <c r="AU26" s="13"/>
-      <c r="AV26" s="13"/>
+      <c r="AS26" s="15">
+        <v>43</v>
+      </c>
+      <c r="AT26" s="15">
+        <v>44</v>
+      </c>
+      <c r="AU26" s="6">
+        <v>45</v>
+      </c>
+      <c r="AV26" s="6">
+        <v>46</v>
+      </c>
       <c r="AW26" s="13"/>
       <c r="AX26" s="13"/>
       <c r="AY26" s="13"/>
@@ -5806,270 +5889,87 @@
       <c r="CF26" s="1"/>
       <c r="CG26" s="1"/>
     </row>
-    <row r="27">
-      <c r="A27" s="19">
-        <v>25</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="24">
-        <v>1</v>
-      </c>
-      <c r="D27" s="25">
-        <v>2</v>
-      </c>
-      <c r="E27" s="1">
-        <v>3</v>
-      </c>
-      <c r="F27" s="24">
-        <v>4</v>
-      </c>
-      <c r="G27" s="15">
-        <v>5</v>
-      </c>
-      <c r="H27" s="26">
-        <v>6</v>
-      </c>
-      <c r="I27" s="24">
-        <v>7</v>
-      </c>
-      <c r="J27" s="26">
-        <v>8</v>
-      </c>
-      <c r="K27" s="16">
-        <v>9</v>
-      </c>
-      <c r="L27" s="24">
-        <v>10</v>
-      </c>
-      <c r="M27" s="26">
-        <v>11</v>
-      </c>
-      <c r="N27" s="24">
-        <v>12</v>
-      </c>
-      <c r="O27" s="15">
-        <v>13</v>
-      </c>
-      <c r="P27" s="16">
-        <v>14</v>
-      </c>
-      <c r="Q27" s="16">
-        <v>15</v>
-      </c>
-      <c r="R27" s="26">
-        <v>16</v>
-      </c>
-      <c r="S27" s="26">
-        <v>17</v>
-      </c>
-      <c r="T27" s="23">
-        <v>18</v>
-      </c>
-      <c r="U27" s="16">
-        <v>19</v>
-      </c>
-      <c r="V27" s="26">
-        <v>20</v>
-      </c>
-      <c r="W27" s="26">
-        <v>21</v>
-      </c>
-      <c r="X27" s="26">
-        <v>22</v>
-      </c>
-      <c r="Y27" s="23">
-        <v>23</v>
-      </c>
-      <c r="Z27" s="15">
-        <v>24</v>
-      </c>
-      <c r="AA27" s="16">
-        <v>25</v>
-      </c>
-      <c r="AB27" s="16">
-        <v>26</v>
-      </c>
-      <c r="AC27" s="16">
+    <row r="28">
+      <c r="B28" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="AD27" s="16">
+      <c r="D28" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AE27" s="26">
-        <v>29</v>
-      </c>
-      <c r="AF27" s="26">
-        <v>30</v>
-      </c>
-      <c r="AG27" s="16">
-        <v>31</v>
-      </c>
-      <c r="AH27" s="16">
-        <v>32</v>
-      </c>
-      <c r="AI27" s="16">
-        <v>33</v>
-      </c>
-      <c r="AJ27" s="16">
-        <v>34</v>
-      </c>
-      <c r="AK27" s="16">
-        <v>35</v>
-      </c>
-      <c r="AL27" s="16">
-        <v>36</v>
-      </c>
-      <c r="AM27" s="16">
-        <v>37</v>
-      </c>
-      <c r="AN27" s="16">
-        <v>38</v>
-      </c>
-      <c r="AO27" s="8">
-        <v>39</v>
-      </c>
-      <c r="AP27" s="8">
-        <v>40</v>
-      </c>
-      <c r="AQ27" s="8">
-        <v>41</v>
-      </c>
-      <c r="AR27" s="8">
-        <v>42</v>
-      </c>
-      <c r="AS27" s="15">
-        <v>43</v>
-      </c>
-      <c r="AT27" s="15">
-        <v>44</v>
-      </c>
-      <c r="AU27" s="6">
-        <v>45</v>
-      </c>
-      <c r="AV27" s="6">
-        <v>46</v>
-      </c>
-      <c r="AW27" s="13"/>
-      <c r="AX27" s="13"/>
-      <c r="AY27" s="13"/>
-      <c r="AZ27" s="13"/>
-      <c r="BA27" s="13"/>
-      <c r="BB27" s="13"/>
-      <c r="BC27" s="13"/>
-      <c r="BD27" s="13"/>
-      <c r="BE27" s="13"/>
-      <c r="BF27" s="13"/>
-      <c r="BG27" s="13"/>
-      <c r="BH27" s="13"/>
-      <c r="BI27" s="13"/>
-      <c r="BJ27" s="13"/>
-      <c r="BK27" s="13"/>
-      <c r="BL27" s="13"/>
-      <c r="BM27" s="13"/>
-      <c r="BN27" s="13"/>
-      <c r="BO27" s="13"/>
-      <c r="BP27" s="1"/>
-      <c r="BQ27" s="1"/>
-      <c r="BR27" s="1"/>
-      <c r="BS27" s="1"/>
-      <c r="BT27" s="1"/>
-      <c r="BU27" s="1"/>
-      <c r="BV27" s="1"/>
-      <c r="BW27" s="1"/>
-      <c r="BX27" s="1"/>
-      <c r="BY27" s="1"/>
-      <c r="BZ27" s="1"/>
-      <c r="CA27" s="1"/>
-      <c r="CB27" s="1"/>
-      <c r="CC27" s="1"/>
-      <c r="CD27" s="1"/>
-      <c r="CE27" s="1"/>
-      <c r="CF27" s="1"/>
-      <c r="CG27" s="1"/>
     </row>
     <row r="29">
       <c r="B29" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="D29" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="C29" s="28"/>
+      <c r="D29" s="29">
+        <v>88</v>
       </c>
     </row>
     <row r="30">
-      <c r="B30" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="28"/>
-      <c r="D30" s="29">
-        <v>88</v>
+      <c r="B30" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="31"/>
+      <c r="D30" s="14">
+        <v>103</v>
       </c>
     </row>
     <row r="31">
-      <c r="B31" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="C31" s="31"/>
+      <c r="B31" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="33"/>
       <c r="D31" s="14">
-        <v>103</v>
+        <v>14</v>
       </c>
     </row>
     <row r="32">
-      <c r="B32" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="C32" s="33"/>
+      <c r="B32" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="34"/>
       <c r="D32" s="14">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C33" s="34"/>
+        <v>33</v>
+      </c>
+      <c r="C33" s="35"/>
       <c r="D33" s="14">
-        <v>31</v>
+        <v>220</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="35"/>
+        <v>34</v>
+      </c>
+      <c r="C34" s="36"/>
       <c r="D34" s="14">
-        <v>220</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C35" s="36"/>
-      <c r="D35" s="14">
-        <v>94</v>
+        <v>35</v>
+      </c>
+      <c r="C35" s="9"/>
+      <c r="D35" s="29">
+        <v>19</v>
       </c>
     </row>
     <row r="36">
-      <c r="B36" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="29">
-        <v>19</v>
+      <c r="C36" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="37">
+        <f>SUM(D29:D35)</f>
+        <v>569</v>
       </c>
     </row>
-    <row r="37">
-      <c r="C37" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="37">
-        <f>SUM(D30:D36)</f>
-        <v>569</v>
-      </c>
-    </row>
-    <row r="38" ht="15.75" customHeight="1"/>
+    <row r="37" ht="15.75" customHeight="1"/>
   </sheetData>
   <printOptions headings="0" gridLines="1" horizontalCentered="1"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>